<commit_message>
add new figs and tables
</commit_message>
<xml_diff>
--- a/docs/StatisticsTest.xlsx
+++ b/docs/StatisticsTest.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\social-predictability\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A521770-173E-4DB6-8BA6-5B0D92CD6F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CEEDEF-4468-48D0-B044-0147EB3AE148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="2355" windowWidth="8325" windowHeight="13485" activeTab="1" xr2:uid="{08454B3E-CBD1-47BE-9BBA-4F7F9312EA2A}"/>
+    <workbookView xWindow="2130" yWindow="855" windowWidth="20145" windowHeight="13485" activeTab="1" xr2:uid="{08454B3E-CBD1-47BE-9BBA-4F7F9312EA2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Spearman" sheetId="1" r:id="rId1"/>
     <sheet name="Wilcoxon" sheetId="2" r:id="rId2"/>
+    <sheet name="H-MFN" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="35">
   <si>
     <t>Weeplace</t>
   </si>
@@ -124,6 +125,21 @@
   </si>
   <si>
     <t>Ranking by MeetupNp</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>Ranking by  FreqNp</t>
+  </si>
+  <si>
+    <t>Ranking by FreqNp</t>
   </si>
 </sst>
 </file>
@@ -133,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +194,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -211,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -284,6 +308,12 @@
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -292,6 +322,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE921E9C-4CC9-4083-9B91-8938B5AD6460}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,18 +655,18 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-    </row>
-    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+    </row>
+    <row r="2" spans="1:7" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -656,8 +689,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -679,8 +712,8 @@
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
@@ -700,8 +733,8 @@
         <v>289</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
@@ -721,8 +754,8 @@
         <v>289</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
@@ -742,8 +775,8 @@
         <v>289</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -765,8 +798,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
       <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
@@ -786,8 +819,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
       <c r="B9" s="6" t="s">
         <v>3</v>
       </c>
@@ -807,8 +840,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
       <c r="B10" s="7" t="s">
         <v>4</v>
       </c>
@@ -828,8 +861,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -851,8 +884,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
       <c r="B12" s="7" t="s">
         <v>2</v>
       </c>
@@ -872,8 +905,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
       <c r="B13" s="6" t="s">
         <v>3</v>
       </c>
@@ -893,8 +926,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
@@ -915,15 +948,15 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -949,7 +982,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -972,7 +1005,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
@@ -993,7 +1026,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
@@ -1014,7 +1047,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1068,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1058,7 +1091,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="3" t="s">
         <v>3</v>
       </c>
@@ -1079,7 +1112,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
@@ -1100,7 +1133,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="3" t="s">
         <v>4</v>
       </c>
@@ -1121,7 +1154,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1144,7 +1177,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
@@ -1165,7 +1198,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="2" t="s">
         <v>1</v>
       </c>
@@ -1186,7 +1219,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="3" t="s">
         <v>4</v>
       </c>
@@ -1203,6 +1236,298 @@
         <v>0.98947399999999996</v>
       </c>
       <c r="G30" s="3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+    </row>
+    <row r="33" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>38</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.57575799999999999</v>
+      </c>
+      <c r="E34" s="2">
+        <v>40</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0.60606099999999996</v>
+      </c>
+      <c r="G34" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="29"/>
+      <c r="B35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="3">
+        <v>41</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0.62121199999999999</v>
+      </c>
+      <c r="E35" s="3">
+        <v>44</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="G35" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="29"/>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2">
+        <v>40</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.60606099999999996</v>
+      </c>
+      <c r="E36" s="2">
+        <v>43</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0.65151499999999996</v>
+      </c>
+      <c r="G36" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="29"/>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3">
+        <v>42</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0.63636400000000004</v>
+      </c>
+      <c r="E37" s="3">
+        <v>45</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0.68181800000000004</v>
+      </c>
+      <c r="G37" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2">
+        <v>128</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.90140799999999999</v>
+      </c>
+      <c r="E38" s="2">
+        <v>131</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0.92253499999999999</v>
+      </c>
+      <c r="G38" s="2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
+      <c r="B39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="3">
+        <v>123</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0.86619699999999999</v>
+      </c>
+      <c r="E39" s="3">
+        <v>127</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.89436599999999999</v>
+      </c>
+      <c r="G39" s="3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="29"/>
+      <c r="B40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <v>120</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0.84506999999999999</v>
+      </c>
+      <c r="E40" s="2">
+        <v>124</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0.87323899999999999</v>
+      </c>
+      <c r="G40" s="2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="29"/>
+      <c r="B41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="3">
+        <v>115</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0.809859</v>
+      </c>
+      <c r="E41" s="3">
+        <v>120</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.84506999999999999</v>
+      </c>
+      <c r="G41" s="3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2">
+        <v>234</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.82105300000000003</v>
+      </c>
+      <c r="E42" s="2">
+        <v>243</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0.85263199999999995</v>
+      </c>
+      <c r="G42" s="2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="29"/>
+      <c r="B43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="3">
+        <v>229</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0.80350900000000003</v>
+      </c>
+      <c r="E43" s="3">
+        <v>236</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0.82806999999999997</v>
+      </c>
+      <c r="G43" s="3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="29"/>
+      <c r="B44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2">
+        <v>234</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.82105300000000003</v>
+      </c>
+      <c r="E44" s="2">
+        <v>239</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0.83859600000000001</v>
+      </c>
+      <c r="G44" s="2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="29"/>
+      <c r="B45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="3">
+        <v>250</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0.877193</v>
+      </c>
+      <c r="E45" s="3">
+        <v>258</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0.90526300000000004</v>
+      </c>
+      <c r="G45" s="3">
         <v>285</v>
       </c>
     </row>
@@ -1211,7 +1536,11 @@
     <sortCondition ref="A19:A30"/>
     <sortCondition ref="B19:B30"/>
   </sortState>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A42:A45"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="A19:A22"/>
@@ -1227,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05316673-4B3D-4F7D-B79F-40BDF0A59593}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,16 +1571,16 @@
     <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+    </row>
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -1268,8 +1597,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1285,8 +1614,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
       <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
@@ -1300,8 +1629,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
       <c r="B5" s="9" t="s">
         <v>19</v>
       </c>
@@ -1315,8 +1644,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
       <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
@@ -1330,8 +1659,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
       <c r="B7" s="9" t="s">
         <v>21</v>
       </c>
@@ -1345,8 +1674,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
       <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
@@ -1360,8 +1689,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -1377,8 +1706,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
       <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
@@ -1392,8 +1721,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
       <c r="B11" s="9" t="s">
         <v>19</v>
       </c>
@@ -1407,8 +1736,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
       <c r="B12" s="9" t="s">
         <v>20</v>
       </c>
@@ -1422,8 +1751,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
       <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
@@ -1437,8 +1766,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
       <c r="B14" s="9" t="s">
         <v>22</v>
       </c>
@@ -1452,8 +1781,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -1469,8 +1798,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
       <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
@@ -1484,8 +1813,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
       <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
@@ -1499,8 +1828,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
       <c r="B18" s="9" t="s">
         <v>20</v>
       </c>
@@ -1514,8 +1843,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="30"/>
       <c r="B19" s="9" t="s">
         <v>21</v>
       </c>
@@ -1529,8 +1858,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
       <c r="B20" s="9" t="s">
         <v>22</v>
       </c>
@@ -1545,13 +1874,13 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
@@ -1571,7 +1900,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -1588,7 +1917,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="9" t="s">
         <v>18</v>
       </c>
@@ -1603,7 +1932,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="21" t="s">
         <v>19</v>
       </c>
@@ -1618,7 +1947,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="21" t="s">
         <v>20</v>
       </c>
@@ -1633,7 +1962,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="9" t="s">
         <v>21</v>
       </c>
@@ -1648,7 +1977,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="9" t="s">
         <v>22</v>
       </c>
@@ -1663,7 +1992,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -1680,7 +2009,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="9" t="s">
         <v>18</v>
       </c>
@@ -1695,7 +2024,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="9" t="s">
         <v>19</v>
       </c>
@@ -1710,7 +2039,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="9" t="s">
         <v>20</v>
       </c>
@@ -1725,7 +2054,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="9" t="s">
         <v>21</v>
       </c>
@@ -1740,7 +2069,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="17" t="s">
         <v>22</v>
       </c>
@@ -1755,7 +2084,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -1772,7 +2101,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="9" t="s">
         <v>18</v>
       </c>
@@ -1787,7 +2116,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="9" t="s">
         <v>19</v>
       </c>
@@ -1802,7 +2131,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
@@ -1817,7 +2146,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="9" t="s">
         <v>21</v>
       </c>
@@ -1832,7 +2161,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="17" t="s">
         <v>22</v>
       </c>
@@ -1844,13 +2173,319 @@
       </c>
       <c r="E42" s="19" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47">
+        <v>82013</v>
+      </c>
+      <c r="D47" s="14">
+        <v>1.748152E-3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="29"/>
+      <c r="B48" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <v>71140</v>
+      </c>
+      <c r="D48" s="15">
+        <v>4.6850389999999998E-4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="29"/>
+      <c r="B49" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49">
+        <v>51386</v>
+      </c>
+      <c r="D49" s="22">
+        <v>9.2502500000000008E-16</v>
+      </c>
+      <c r="E49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="29"/>
+      <c r="B50" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50">
+        <v>37750</v>
+      </c>
+      <c r="D50" s="25">
+        <v>7.7920490000000003E-17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="29"/>
+      <c r="B51" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51">
+        <v>64351</v>
+      </c>
+      <c r="D51" s="14">
+        <v>4.0323650000000001E-13</v>
+      </c>
+      <c r="E51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="29"/>
+      <c r="B52" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52">
+        <v>72712</v>
+      </c>
+      <c r="D52" s="15">
+        <v>4.812975E-4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53">
+        <v>367262</v>
+      </c>
+      <c r="D53" s="14">
+        <v>1.23465E-2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="29"/>
+      <c r="B54" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54">
+        <v>306657</v>
+      </c>
+      <c r="D54" s="15">
+        <v>3.0677189999999998E-11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="29"/>
+      <c r="B55" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55">
+        <v>204885</v>
+      </c>
+      <c r="D55" s="14">
+        <v>1.4060320000000001E-13</v>
+      </c>
+      <c r="E55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="29"/>
+      <c r="B56" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56">
+        <v>190302</v>
+      </c>
+      <c r="D56" s="15">
+        <v>1.4123289999999999E-3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="29"/>
+      <c r="B57" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57">
+        <v>303811</v>
+      </c>
+      <c r="D57" s="14">
+        <v>7.2267889999999997E-9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="29"/>
+      <c r="B58" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58">
+        <v>211001</v>
+      </c>
+      <c r="D58" s="25">
+        <v>6.028795E-38</v>
+      </c>
+      <c r="E58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59">
+        <v>1329611</v>
+      </c>
+      <c r="D59" s="14">
+        <v>9.3109159999999994E-13</v>
+      </c>
+      <c r="E59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="29"/>
+      <c r="B60" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60">
+        <v>1319038</v>
+      </c>
+      <c r="D60" s="15">
+        <v>2.4225019999999998E-10</v>
+      </c>
+      <c r="E60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="29"/>
+      <c r="B61" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61">
+        <v>662844</v>
+      </c>
+      <c r="D61" s="14">
+        <v>2.15565E-66</v>
+      </c>
+      <c r="E61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="29"/>
+      <c r="B62" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62">
+        <v>861454</v>
+      </c>
+      <c r="D62" s="15">
+        <v>1.135243E-4</v>
+      </c>
+      <c r="E62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="29"/>
+      <c r="B63" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63">
+        <v>1344301</v>
+      </c>
+      <c r="D63" s="14">
+        <v>2.4512029999999998E-4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="29"/>
+      <c r="B64" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64">
+        <v>1135244</v>
+      </c>
+      <c r="D64" s="25">
+        <v>4.6027289999999995E-16</v>
+      </c>
+      <c r="E64" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:E42">
     <sortCondition ref="A25:A42"/>
   </sortState>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A59:A64"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A1:E1"/>
@@ -1862,4 +2497,232 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B139C033-AA48-4953-AD8F-5122EF37AD9E}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+    </row>
+    <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>141</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.83431952662721898</v>
+      </c>
+      <c r="E3" s="2">
+        <v>144</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.85207100591715901</v>
+      </c>
+      <c r="G3" s="2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>222</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>229</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="G4" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>694</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.92410119840213001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>700</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.93209054593874796</v>
+      </c>
+      <c r="G5" s="2">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" spans="1:7" ht="48" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>96</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.56804733727810597</v>
+      </c>
+      <c r="E11" s="2">
+        <v>100</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.59171597633136097</v>
+      </c>
+      <c r="G11" s="2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>208</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="E12" s="2">
+        <v>216</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>585</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.77896138482023902</v>
+      </c>
+      <c r="E13" s="2">
+        <v>602</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.80159786950732304</v>
+      </c>
+      <c r="G13" s="2">
+        <v>751</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>